<commit_message>
Added batch 2 data sheets
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_SNG_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_SNG_REGRESSION.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\BAU\GlobalTestSuiteAutomation\WppRegPack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Documents\Results\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -25,48 +25,51 @@
     <sheet name="UserCreation" sheetId="6" r:id="rId11"/>
     <sheet name="EmployeeAsUser" sheetId="7" r:id="rId12"/>
     <sheet name="ChangeEmployee" sheetId="25" r:id="rId13"/>
-    <sheet name="ChangeUser" sheetId="43" r:id="rId14"/>
-    <sheet name="Modify budget" sheetId="32" r:id="rId15"/>
-    <sheet name="CreateQuote" sheetId="16" r:id="rId16"/>
-    <sheet name="Approve Expenses Sheet Opco" sheetId="29" r:id="rId17"/>
-    <sheet name="Approve Expenses Sheet SSC" sheetId="30" r:id="rId18"/>
-    <sheet name="Reject Expenses" sheetId="31" r:id="rId19"/>
-    <sheet name="ApproveTimesheet" sheetId="17" r:id="rId20"/>
-    <sheet name="RejectTimesheet" sheetId="18" r:id="rId21"/>
-    <sheet name="FixedAssetPurchaseOrder" sheetId="19" r:id="rId22"/>
-    <sheet name="CreatePurchaseOrder" sheetId="15" r:id="rId23"/>
-    <sheet name="ApprovePurchaseOrder" sheetId="20" r:id="rId24"/>
-    <sheet name="RejectPurchaseOrder" sheetId="21" r:id="rId25"/>
-    <sheet name="Create Fixed Asset" sheetId="34" r:id="rId26"/>
-    <sheet name="FixedAssetDepreciation" sheetId="33" r:id="rId27"/>
-    <sheet name="FixedAssetVal" sheetId="26" r:id="rId28"/>
-    <sheet name="FixedAssetDisposal" sheetId="27" r:id="rId29"/>
-    <sheet name="PostEntries" sheetId="28" r:id="rId30"/>
-    <sheet name="VendorInvoice" sheetId="22" r:id="rId31"/>
-    <sheet name="ApproveVendorInvoice" sheetId="23" r:id="rId32"/>
-    <sheet name="RejectVendorInvoice" sheetId="24" r:id="rId33"/>
-    <sheet name="PostVendorJournal" sheetId="44" r:id="rId34"/>
-    <sheet name="AR Single Payment" sheetId="35" r:id="rId35"/>
-    <sheet name="AR Multiple Payment" sheetId="36" r:id="rId36"/>
-    <sheet name="Post a Customer Payment" sheetId="37" r:id="rId37"/>
-    <sheet name="Post in Foreign currency" sheetId="38" r:id="rId38"/>
-    <sheet name="Writingoffbad" sheetId="39" r:id="rId39"/>
-    <sheet name="Reverse a Credit Note" sheetId="40" r:id="rId40"/>
-    <sheet name="Reverse Invoice" sheetId="41" r:id="rId41"/>
-    <sheet name="Credit Note With PO" sheetId="42" r:id="rId42"/>
-    <sheet name="CreateClient" sheetId="49" r:id="rId43"/>
-    <sheet name="AmendGlobalClient" sheetId="50" r:id="rId44"/>
-    <sheet name="AmendGlobalBrand" sheetId="51" r:id="rId45"/>
-    <sheet name="BlockGlobalClient" sheetId="48" r:id="rId46"/>
-    <sheet name="BlockGlobalBrand" sheetId="47" r:id="rId47"/>
-    <sheet name="CreateGeneralJournal" sheetId="52" r:id="rId48"/>
-    <sheet name="ReverseGL" sheetId="53" r:id="rId49"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId50"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId51"/>
+    <sheet name="ReallocateJobEntries" sheetId="54" r:id="rId14"/>
+    <sheet name="JobClosure" sheetId="55" r:id="rId15"/>
+    <sheet name="BlockUser" sheetId="56" r:id="rId16"/>
+    <sheet name="ChangeUser" sheetId="43" r:id="rId17"/>
+    <sheet name="Modify budget" sheetId="32" r:id="rId18"/>
+    <sheet name="CreateQuote" sheetId="16" r:id="rId19"/>
+    <sheet name="Approve Expenses Sheet Opco" sheetId="29" r:id="rId20"/>
+    <sheet name="Approve Expenses Sheet SSC" sheetId="30" r:id="rId21"/>
+    <sheet name="Reject Expenses" sheetId="31" r:id="rId22"/>
+    <sheet name="ApproveTimesheet" sheetId="17" r:id="rId23"/>
+    <sheet name="RejectTimesheet" sheetId="18" r:id="rId24"/>
+    <sheet name="FixedAssetPurchaseOrder" sheetId="19" r:id="rId25"/>
+    <sheet name="CreatePurchaseOrder" sheetId="15" r:id="rId26"/>
+    <sheet name="ApprovePurchaseOrder" sheetId="20" r:id="rId27"/>
+    <sheet name="RejectPurchaseOrder" sheetId="21" r:id="rId28"/>
+    <sheet name="Create Fixed Asset" sheetId="34" r:id="rId29"/>
+    <sheet name="FixedAssetDepreciation" sheetId="33" r:id="rId30"/>
+    <sheet name="FixedAssetVal" sheetId="26" r:id="rId31"/>
+    <sheet name="FixedAssetDisposal" sheetId="27" r:id="rId32"/>
+    <sheet name="PostEntries" sheetId="28" r:id="rId33"/>
+    <sheet name="VendorInvoice" sheetId="22" r:id="rId34"/>
+    <sheet name="ApproveVendorInvoice" sheetId="23" r:id="rId35"/>
+    <sheet name="RejectVendorInvoice" sheetId="24" r:id="rId36"/>
+    <sheet name="PostVendorJournal" sheetId="44" r:id="rId37"/>
+    <sheet name="AR Single Payment" sheetId="35" r:id="rId38"/>
+    <sheet name="AR Multiple Payment" sheetId="36" r:id="rId39"/>
+    <sheet name="Post a Customer Payment" sheetId="37" r:id="rId40"/>
+    <sheet name="Post in Foreign currency" sheetId="38" r:id="rId41"/>
+    <sheet name="Writingoffbad" sheetId="39" r:id="rId42"/>
+    <sheet name="Reverse a Credit Note" sheetId="40" r:id="rId43"/>
+    <sheet name="Reverse Invoice" sheetId="41" r:id="rId44"/>
+    <sheet name="Credit Note With PO" sheetId="42" r:id="rId45"/>
+    <sheet name="CreateClient" sheetId="49" r:id="rId46"/>
+    <sheet name="AmendGlobalClient" sheetId="50" r:id="rId47"/>
+    <sheet name="AmendGlobalBrand" sheetId="51" r:id="rId48"/>
+    <sheet name="BlockGlobalClient" sheetId="48" r:id="rId49"/>
+    <sheet name="BlockGlobalBrand" sheetId="47" r:id="rId50"/>
+    <sheet name="CreateGeneralJournal" sheetId="52" r:id="rId51"/>
+    <sheet name="ReverseGL" sheetId="53" r:id="rId52"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId53"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId54"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -74,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="1157">
   <si>
     <t>Description</t>
   </si>
@@ -3506,17 +3509,52 @@
     <t>E1005</t>
   </si>
   <si>
-    <t>1517101146</t>
-  </si>
-  <si>
     <t>1517101149</t>
+  </si>
+  <si>
+    <t>1216-Grey Shopper DPI Limited</t>
+  </si>
+  <si>
+    <t>1289-Red Wasabi Marketing Consulting (Shanghai) Co. Ltd</t>
+  </si>
+  <si>
+    <t>RJ_Autom_01</t>
+  </si>
+  <si>
+    <t>1201_TestAutomationJob</t>
+  </si>
+  <si>
+    <t>1216-Retainer Auto Job</t>
+  </si>
+  <si>
+    <t>1289-FPCP job</t>
+  </si>
+  <si>
+    <t>1307200405</t>
+  </si>
+  <si>
+    <t>NewJob_No</t>
+  </si>
+  <si>
+    <t>1307200406</t>
+  </si>
+  <si>
+    <t>1307_TestAutomationJob 14October2019 13:53:34</t>
+  </si>
+  <si>
+    <t>1307_AutomationUser 18October2019 15:21:12</t>
+  </si>
+  <si>
+    <t>11/30/2019</t>
+  </si>
+  <si>
+    <t>1307_TestEmployeeAutomation 11October2019 11:26:39</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3803,7 +3841,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4004,6 +4042,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4296,8 +4352,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="9" bestFit="true" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="9" width="40.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4367,16 +4423,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="31.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="60.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="30" width="59.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="30" width="51.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="30" width="51.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="30" width="58.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="30" width="57.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="30" width="63.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="30" width="45.28515625" collapsed="true"/>
-    <col min="10" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="31" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="59.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="51" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.85546875" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="58.140625" style="30" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="57.7109375" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="63.7109375" style="30" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.28515625" style="30" customWidth="1" collapsed="1"/>
+    <col min="10" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5045,9 +5101,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="30" width="23.140625" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.140625" style="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5144,11 +5200,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="68.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="67.42578125" collapsed="true"/>
-    <col min="4" max="9" bestFit="true" customWidth="true" width="87.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="69.42578125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="9" width="87.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="69.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5995,8 +6051,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="31.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="60.140625" collapsed="true"/>
+    <col min="1" max="1" width="31" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6115,6 +6171,331 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1307</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1201</v>
+      </c>
+      <c r="D1" s="104">
+        <v>1216</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1307</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1201</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1216</v>
+      </c>
+      <c r="E2" s="105">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="107" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="108" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="108" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1307</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1201</v>
+      </c>
+      <c r="D1" s="104">
+        <v>1216</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1307</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1201</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1216</v>
+      </c>
+      <c r="E2" s="105">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="106" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="107" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="50">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="109" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="51">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="51">
+        <v>130710080</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="51">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
+        <v>305</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:B9"/>
@@ -6125,7 +6506,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6204,7 +6585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -6217,9 +6598,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.25">
@@ -6507,182 +6888,6 @@
       </c>
       <c r="N4">
         <v>1500</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C1" s="31">
-        <v>1322</v>
-      </c>
-      <c r="D1" s="31">
-        <v>1319</v>
-      </c>
-      <c r="E1" s="31">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="60"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>304</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>345</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>346</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>345</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1307</v>
-      </c>
-      <c r="B2">
-        <v>1307</v>
-      </c>
-      <c r="C2">
-        <v>1307700041</v>
-      </c>
-      <c r="D2" t="s">
-        <v>349</v>
-      </c>
-      <c r="E2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F2" t="s">
-        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -6696,40 +6901,56 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="31">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>345</v>
-      </c>
-      <c r="B3">
-        <v>1307700044</v>
+      <c r="B1" s="31" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C1" s="31">
+        <v>1322</v>
+      </c>
+      <c r="D1" s="31">
+        <v>1319</v>
+      </c>
+      <c r="E1" s="31">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="60"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6751,10 +6972,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="23.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="30" width="27.85546875" collapsed="true"/>
-    <col min="3" max="155" customWidth="true" style="30" width="32.0" collapsed="true"/>
-    <col min="156" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="23.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" style="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="155" width="32" style="30" customWidth="1" collapsed="1"/>
+    <col min="156" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:155" x14ac:dyDescent="0.25">
@@ -6923,7 +7144,7 @@
         <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="3" spans="1:155" x14ac:dyDescent="0.25">
@@ -6982,6 +7203,166 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1307</v>
+      </c>
+      <c r="B2">
+        <v>1307</v>
+      </c>
+      <c r="C2">
+        <v>1307700041</v>
+      </c>
+      <c r="D2" t="s">
+        <v>349</v>
+      </c>
+      <c r="E2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="31">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="B3">
+        <v>1307700044</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -6994,8 +7375,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7032,7 +7413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7045,8 +7426,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7083,7 +7464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7096,48 +7477,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -7310,7 +7691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7323,39 +7704,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="15.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" width="15.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
@@ -7523,7 +7904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7536,8 +7917,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7578,7 +7959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7591,8 +7972,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7635,7 +8016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7648,8 +8029,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7714,221 +8095,6 @@
       </c>
       <c r="B8" t="s">
         <v>364</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="21.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="22.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="30" width="12.42578125" collapsed="true"/>
-    <col min="4" max="16384" style="30" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>355</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>356</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>357</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>335</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1307</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>329</v>
-      </c>
-      <c r="B3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>331</v>
-      </c>
-      <c r="B4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
-        <v>333</v>
-      </c>
-      <c r="B5" s="77" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
-        <v>335</v>
-      </c>
-      <c r="B6" s="77" t="s">
-        <v>336</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="63" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
-        <v>331</v>
-      </c>
-      <c r="B2" s="78" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
-        <v>337</v>
-      </c>
-      <c r="B3" s="85" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
-        <v>339</v>
-      </c>
-      <c r="B4" s="77" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
-        <v>340</v>
-      </c>
-      <c r="B5" s="78" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
-        <v>342</v>
-      </c>
-      <c r="B6" s="79" t="s">
-        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -7950,7 +8116,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="12.0" collapsed="true"/>
+    <col min="2" max="2" width="12" style="30" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -9127,61 +9293,63 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="21.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="80" t="s">
-        <v>74</v>
+      <c r="A1" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1">
+        <v>1307</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
-        <v>328</v>
-      </c>
-      <c r="B2" s="86" t="s">
-        <v>74</v>
+      <c r="A2" s="30" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
-        <v>329</v>
-      </c>
-      <c r="B3" s="86" t="s">
-        <v>330</v>
+      <c r="A3" s="30" t="s">
+        <v>356</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>846</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
-        <v>331</v>
-      </c>
-      <c r="B4" s="81" t="s">
-        <v>332</v>
+      <c r="A4" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
-        <v>333</v>
-      </c>
-      <c r="B5" s="82" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="83" t="s">
+      <c r="A5" s="30" t="s">
         <v>335</v>
       </c>
-      <c r="B6" s="84" t="s">
-        <v>336</v>
+      <c r="B5" s="30" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1307</v>
       </c>
     </row>
   </sheetData>
@@ -9191,6 +9359,219 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="75" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="77" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="75" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" s="77" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="75" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
+        <v>337</v>
+      </c>
+      <c r="B3" s="85" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" s="77" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" s="79" t="s">
+        <v>343</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="86" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="81" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="82" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="83" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" s="84" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -9203,11 +9584,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="7" max="15" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="15" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -9314,7 +9695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -9327,7 +9708,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -9361,7 +9742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -9374,7 +9755,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -9391,217 +9772,6 @@
       </c>
       <c r="B2" s="59" t="s">
         <v>836</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.42578125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>404</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="24.42578125" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="30">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>367</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>368</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>369</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>367</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>370</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="B2" s="30">
-        <v>1307</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>380</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>381</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>382</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>369</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -9618,45 +9788,45 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1">
+      <c r="A1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2">
         <v>1307</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="30">
-        <v>1307</v>
+      <c r="B3" s="59" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>380</v>
+      <c r="A4" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -9670,85 +9840,73 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="16.42578125" collapsed="true"/>
-    <col min="2" max="2" style="30" width="9.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="30" width="11.7109375" collapsed="true"/>
-    <col min="4" max="8" style="30" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="30" width="16.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="30" width="27.5703125" collapsed="true"/>
-    <col min="11" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>311</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>367</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>370</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>371</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>372</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
-        <v>180</v>
       </c>
       <c r="B2" s="30">
         <v>1307</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>373</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>374</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>375</v>
-      </c>
-      <c r="F2" s="30" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>368</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>369</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>376</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>377</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>378</v>
-      </c>
-      <c r="J2" s="30" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -9762,23 +9920,20 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>311</v>
       </c>
@@ -9786,66 +9941,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>383</v>
+        <v>208</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>384</v>
-      </c>
-      <c r="F1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G1" t="s">
-        <v>849</v>
-      </c>
-      <c r="H1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="K1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E1" s="30" t="s">
+        <v>367</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>370</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2" t="s">
-        <v>851</v>
-      </c>
-      <c r="E2" t="s">
-        <v>388</v>
-      </c>
-      <c r="F2" t="s">
-        <v>389</v>
-      </c>
-      <c r="G2">
-        <v>111398</v>
-      </c>
-      <c r="H2" t="s">
-        <v>852</v>
-      </c>
-      <c r="I2">
-        <v>1307200433</v>
-      </c>
-      <c r="J2" t="s">
-        <v>853</v>
-      </c>
-      <c r="K2">
-        <v>1000</v>
+        <v>180</v>
+      </c>
+      <c r="B2" s="30">
+        <v>1307</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -9867,7 +10004,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11909,6 +12046,250 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.140625" style="30" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="8" width="9.140625" style="30" collapsed="1"/>
+    <col min="9" max="9" width="16" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="30" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>367</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>370</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>371</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>372</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="30">
+        <v>1307</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>374</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>375</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>376</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F1" t="s">
+        <v>385</v>
+      </c>
+      <c r="G1" t="s">
+        <v>849</v>
+      </c>
+      <c r="H1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>850</v>
+      </c>
+      <c r="K1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2" t="s">
+        <v>851</v>
+      </c>
+      <c r="E2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G2">
+        <v>111398</v>
+      </c>
+      <c r="H2" t="s">
+        <v>852</v>
+      </c>
+      <c r="I2">
+        <v>1307200433</v>
+      </c>
+      <c r="J2" t="s">
+        <v>853</v>
+      </c>
+      <c r="K2">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -11921,9 +12302,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="15.28515625" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11988,7 +12369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -12001,8 +12382,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -12059,7 +12440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
@@ -12072,11 +12453,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -12245,7 +12626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -12258,8 +12639,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -12452,7 +12833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -12465,7 +12846,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -12526,7 +12907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
@@ -12539,8 +12920,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -12604,226 +12985,6 @@
       </c>
       <c r="B10" t="s">
         <v>1068</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="14.140625" collapsed="true"/>
-    <col min="2" max="16384" style="30" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="94" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" t="s">
-        <v>735</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B4:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="30" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="10.0" collapsed="true"/>
-    <col min="3" max="16384" style="30" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="94" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>870</v>
-      </c>
-      <c r="B2" s="60"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>871</v>
-      </c>
-      <c r="B4" s="95"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>872</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1106</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1107</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E1" t="s">
-        <v>384</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1111</v>
-      </c>
-      <c r="H1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1112</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1113</v>
-      </c>
-      <c r="K1" t="s">
-        <v>385</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1115</v>
-      </c>
-      <c r="N1" t="s">
-        <v>137</v>
-      </c>
-      <c r="O1" t="s">
-        <v>1116</v>
-      </c>
-      <c r="P1" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1517</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1123</v>
-      </c>
-      <c r="E2" t="s">
-        <v>389</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1120</v>
-      </c>
-      <c r="H2" s="59" t="s">
-        <v>1118</v>
-      </c>
-      <c r="I2" s="59"/>
-      <c r="J2">
-        <v>500</v>
-      </c>
-      <c r="K2" t="s">
-        <v>389</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1121</v>
-      </c>
-      <c r="N2" s="59" t="s">
-        <v>1119</v>
-      </c>
-      <c r="O2">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -12840,41 +13001,39 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="99" width="18.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="99" width="35.0" collapsed="true"/>
-    <col min="3" max="16384" style="99" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="94" t="s">
         <v>1100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B2" s="101"/>
+      <c r="A2" s="30" t="s">
+        <v>870</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="99" t="s">
-        <v>1126</v>
-      </c>
-      <c r="B3" s="100" t="s">
-        <v>1125</v>
+      <c r="A3" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" t="s">
+        <v>735</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12891,8 +13050,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="33.5703125" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -13048,6 +13207,228 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B4:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="30" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="94" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>870</v>
+      </c>
+      <c r="B2" s="60"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>871</v>
+      </c>
+      <c r="B4" s="95"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>872</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="E1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="H1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="K1" t="s">
+        <v>385</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="N1" t="s">
+        <v>137</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1517</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>1118</v>
+      </c>
+      <c r="I2" s="59"/>
+      <c r="J2">
+        <v>500</v>
+      </c>
+      <c r="K2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>1119</v>
+      </c>
+      <c r="O2">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" style="99" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35" style="99" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="99" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="99" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B2" s="101"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="99" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B3" s="100" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -13060,8 +13441,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -13158,12 +13539,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -13171,9 +13552,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13315,10 +13696,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="49" width="30.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="49" width="33.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="4" max="16384" style="30" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="30.140625" style="49" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" style="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="30" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -13524,39 +13905,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -13850,47 +14231,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -14092,9 +14473,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="30" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed password for 1707 Finance login in Ind_regression sheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Regression/DS_SNG_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Regression/DS_SNG_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Music\SIT-W1_Datasheets\New folder\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Documents\Results\Bau_Environment\GlobalTestSuiteAutomation\WppRegpack\TestResource\Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="20" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="46" activeTab="49"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -7316,7 +7316,7 @@
   </sheetPr>
   <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -12257,7 +12257,7 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -13059,14 +13059,14 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>